<commit_message>
Particle Swarm examples in Matlab
</commit_message>
<xml_diff>
--- a/Lectures/Ex1-GeneticAlgorithm.xlsx
+++ b/Lectures/Ex1-GeneticAlgorithm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Classes\CEE6410\Fall2020\CEE6410-Rosenberg-GitHub\CEE-6410-Rosenberg\Lectures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB2629D-4E54-4EAB-9DB8-1E06AAC9241C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C02B6FE-350D-4629-A93A-2500F05BE7EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8150" xr2:uid="{DAA2575D-E802-404F-A6D7-17C0C9378B1B}"/>
   </bookViews>
@@ -16,16 +16,16 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$C$12:$C$13</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$C$11:$C$12</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.1</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$C$12</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$C$12</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Sheet1!$C$13</definedName>
-    <definedName name="solver_lhs4" localSheetId="0" hidden="1">Sheet1!$C$13</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$C$11</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$C$11</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Sheet1!$C$12</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">Sheet1!$C$12</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.05</definedName>
@@ -34,7 +34,7 @@
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$D$9</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$D$8</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
@@ -680,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6F64C43-BA86-4705-A3B8-DA62AA9771EA}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -717,69 +717,69 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="6">
-        <f>3*(1-C12)^2*EXP(-(C12^2)-(C13+1)^2)-10*(C12/5-C12^3-C13^5)*EXP(-(C12^2)-C13^2)-1/3*EXP(-((C12+1)^2)-C13^2)</f>
-        <v>0.98101184312384626</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="28" x14ac:dyDescent="0.35">
+      <c r="D8" s="6">
+        <f>3*(1-C11)^2*EXP(-(C11^2)-(C12+1)^2)-10*(C11/5-C11^3-C12^5)*EXP(-(C11^2)-C12^2)-1/3*EXP(-((C11+1)^2)-C12^2)</f>
+        <v>8.0283206579095339</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28" x14ac:dyDescent="0.35">
+      <c r="D9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="D10" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>10</v>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="5">
+        <v>-9.3571647733101004E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B12" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C12" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="5">
-        <v>0</v>
+        <v>1.6154467277351743</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>11</v>
+      <c r="A15" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>